<commit_message>
Windows: correct save to excel for multiple samples
</commit_message>
<xml_diff>
--- a/DATA/UKSAF/STO_2doublets.xlsx
+++ b/DATA/UKSAF/STO_2doublets.xlsx
@@ -293,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -350,6 +350,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -17828,7 +17831,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE9"/>
+  <dimension ref="B2:AE9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17869,7 +17872,6 @@
     <col width="6" customWidth="1" min="31" max="31"/>
   </cols>
   <sheetData>
-    <row r="1"/>
     <row r="2">
       <c r="B2" s="21" t="inlineStr">
         <is>

</xml_diff>